<commit_message>
nan and chi and tapi
</commit_message>
<xml_diff>
--- a/R/chi/parameter แต่ละช่วงเดือน.xlsx
+++ b/R/chi/parameter แต่ละช่วงเดือน.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="-105" windowWidth="25605" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,11 +325,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -658,18 +653,12 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="5.25" customWidth="1"/>
-    <col min="3" max="3" width="4.75" customWidth="1"/>
-    <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="4.75" customWidth="1"/>
-    <col min="6" max="6" width="4.125" customWidth="1"/>
-    <col min="7" max="8" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>